<commit_message>
feat: Suite v4.0 Final - Doble Dashboard interactivo (Ventas y Ofertas), Motor BI con limpieza de SKU (mata-ceros), ETL automático a Excel y optimización de foco en PuTTY.
</commit_message>
<xml_diff>
--- a/procesados/stock/MANAOS CARGA.xlsx
+++ b/procesados/stock/MANAOS CARGA.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Suite\Excel_Entrada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Suite_Andres\Excel_Entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4D10EC-4999-4C44-80CF-0208DB1004CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD135D-03F2-4FC7-AAAF-CE0D8DC74F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -359,86 +362,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>965</v>
-      </c>
-      <c r="B1">
-        <f>240*6</f>
-        <v>1440</v>
-      </c>
-      <c r="C1">
-        <v>70527</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>9981</v>
+        <v>940</v>
       </c>
       <c r="B2">
-        <f>240*12</f>
-        <v>2880</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
+        <v>2400</v>
+      </c>
+      <c r="C2">
+        <v>70598</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>970</v>
+        <v>941</v>
       </c>
       <c r="B3">
-        <v>168</v>
+        <v>1920</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="B4">
-        <f>400*6</f>
-        <v>2400</v>
+        <v>1920</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="B5">
-        <f>320*6</f>
         <v>1920</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>944</v>
+        <v>970</v>
       </c>
       <c r="B6">
-        <f>320*6</f>
-        <v>1920</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>965</v>
+      </c>
+      <c r="B7">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>9402</v>
+      </c>
+      <c r="B8">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>946</v>
+      </c>
+      <c r="B9">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>950</v>
+      </c>
+      <c r="B10">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>920</v>
       </c>
-      <c r="B7">
-        <f>75*6</f>
+      <c r="B11">
         <v>450</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>